<commit_message>
Added More README Data
</commit_message>
<xml_diff>
--- a/README_data/Time_Acc_Data.xlsx
+++ b/README_data/Time_Acc_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\SMU\Classes\Spring 2022\CS 3353 (Algorithms)\22s-pa03-girvan-newman-uwunary-tree\README_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE0813-9C31-49F8-BDF9-67BCFCEF4059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E406AA0-9C2A-4F55-AEE2-B7F6F9135948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{E3BB0DCF-3EF3-4353-951C-EAD6C2F98100}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,37 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
-  <si>
-    <t>dataset1</t>
-  </si>
-  <si>
-    <t>dataset2</t>
-  </si>
-  <si>
-    <t>dataset3</t>
-  </si>
-  <si>
-    <t>dataset4</t>
-  </si>
-  <si>
-    <t>dataset5</t>
-  </si>
-  <si>
-    <t>dataset6</t>
-  </si>
-  <si>
-    <t>dataset7</t>
-  </si>
-  <si>
-    <t>dataset8</t>
-  </si>
-  <si>
-    <t>dataset9</t>
-  </si>
-  <si>
-    <t>dataset10</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Dataset</t>
   </si>
@@ -144,6 +113,9 @@
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1239,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -4613,6 +4584,2050 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Number of Out Edges Vs. Algorithm Accuracy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GN (80%)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$29:$B$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.9869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91669999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.83850000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58850000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99217999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.36980000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.11E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>64,32,16,8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$29:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.96875</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.828125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.39319999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70299999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.53900000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.39839999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38279999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$29:$D$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.84379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67190000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2969</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.84379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3594</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,64,32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$29:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99209999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.41410000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38279999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.96089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.60160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52339999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.36720000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,64,32,16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$29:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.97660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.57030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>256,128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$29:$G$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89839999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32029999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92190000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$29:$H$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.40629999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3281</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.35160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.35160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3281</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.28129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30470000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.39529999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024,512,256,128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$29:$I$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.98399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2969</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.80469999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41410000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="336675887"/>
+        <c:axId val="336686703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="336675887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Number Of Out Edges</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="336686703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="336686703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Algorithm Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="336675887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="8"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="9"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="10"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="11"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="12"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="13"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="14"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="15"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Average Number of Out Edges Vs. Average Accuracy Across</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Algorithms</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$29:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.91238124999999992</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88119062500000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71809999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53873749999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.34338125000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30533749999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.84764750000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69825000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.42666249999999994</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33074999999999993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-B16A-4507-B8CA-7C33DEDEC1F5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="336675887"/>
+        <c:axId val="336686703"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="336675887"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Number Of Out Edges</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="336686703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="336686703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Across All Algorithms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="336675887"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4773,6 +6788,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6787,20 +8882,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>174624</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>63226</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>44176</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6827,16 +9954,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>149224</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>73024</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>82549</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6863,16 +9990,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>130175</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>149225</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>492125</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6902,15 +10029,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>168274</xdr:rowOff>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>174624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>169333</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>126999</xdr:rowOff>
+      <xdr:colOff>112183</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6930,6 +10057,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53974</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>96307</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29FD7D0D-9A57-46EB-A6CA-0FAB516A9F9F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>42333</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17607EBB-1FB9-43AB-A1C1-D693E7551CE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7235,10 +10436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA28095E-13BC-4864-999E-18B5B8AAC3DA}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7255,30 +10456,30 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>15.84375</v>
@@ -7301,7 +10502,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>15.9375</v>
@@ -7324,7 +10525,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>16.140625</v>
@@ -7347,7 +10548,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>16.125</v>
@@ -7370,7 +10571,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>16.046875</v>
@@ -7393,7 +10594,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>15.59375</v>
@@ -7416,7 +10617,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B8">
         <v>16.265625</v>
@@ -7439,7 +10640,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B9">
         <v>16.703125</v>
@@ -7462,7 +10663,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>15.859375</v>
@@ -7485,7 +10686,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>16</v>
@@ -7508,27 +10709,27 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
         <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
       </c>
       <c r="G15" s="1">
         <v>256128</v>
@@ -7537,12 +10738,12 @@
         <v>512256</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>7.3239999999999998</v>
@@ -7569,9 +10770,9 @@
         <v>1.9490000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>37.32</v>
@@ -7598,9 +10799,9 @@
         <v>2.077</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>38.468699999999998</v>
@@ -7627,9 +10828,9 @@
         <v>1.9259999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>43.039000000000001</v>
@@ -7656,9 +10857,9 @@
         <v>1.9750000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>33.281999999999996</v>
@@ -7685,9 +10886,9 @@
         <v>1.9550000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>34.5</v>
@@ -7714,9 +10915,9 @@
         <v>1.946</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>36.298699999999997</v>
@@ -7743,9 +10944,9 @@
         <v>1.946</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>44.28</v>
@@ -7772,9 +10973,9 @@
         <v>1.9219999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>33.74</v>
@@ -7801,9 +11002,9 @@
         <v>1.9470000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>37.659999999999997</v>
@@ -7830,29 +11031,29 @@
         <v>2.0590000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" t="s">
         <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
       </c>
       <c r="G28" s="1">
         <v>256128</v>
@@ -7861,12 +11062,15 @@
         <v>512256</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
+      </c>
+      <c r="J28" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B29">
         <v>0.9869</v>
@@ -7892,10 +11096,14 @@
       <c r="I29">
         <v>0.98399999999999999</v>
       </c>
+      <c r="J29">
+        <f>AVERAGE(B29:I29)</f>
+        <v>0.91238124999999992</v>
+      </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B30">
         <v>0.91669999999999996</v>
@@ -7921,10 +11129,14 @@
       <c r="I30">
         <v>1</v>
       </c>
+      <c r="J30">
+        <f t="shared" ref="J30:J38" si="0">AVERAGE(B30:I30)</f>
+        <v>0.88119062500000001</v>
+      </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B31">
         <v>0.83850000000000002</v>
@@ -7950,10 +11162,14 @@
       <c r="I31">
         <v>0.96089999999999998</v>
       </c>
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>0.71809999999999996</v>
+      </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B32">
         <v>0.58850000000000002</v>
@@ -7979,10 +11195,14 @@
       <c r="I32">
         <v>0.63280000000000003</v>
       </c>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>0.53873749999999998</v>
+      </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B33">
         <v>0.15625</v>
@@ -8008,10 +11228,14 @@
       <c r="I33">
         <v>0.2969</v>
       </c>
+      <c r="J33">
+        <f t="shared" si="0"/>
+        <v>0.34338125000000003</v>
+      </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B34">
         <v>0.125</v>
@@ -8037,10 +11261,14 @@
       <c r="I34">
         <v>0.375</v>
       </c>
+      <c r="J34">
+        <f t="shared" si="0"/>
+        <v>0.30533749999999998</v>
+      </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B35">
         <v>0.99217999999999995</v>
@@ -8066,10 +11294,14 @@
       <c r="I35">
         <v>0.99219999999999997</v>
       </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>0.84764750000000011</v>
+      </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B36">
         <v>0.96089999999999998</v>
@@ -8095,10 +11327,14 @@
       <c r="I36">
         <v>0.80469999999999997</v>
       </c>
+      <c r="J36">
+        <f t="shared" si="0"/>
+        <v>0.69825000000000004</v>
+      </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B37">
         <v>0.36980000000000002</v>
@@ -8124,10 +11360,14 @@
       <c r="I37">
         <v>0.55449999999999999</v>
       </c>
+      <c r="J37">
+        <f t="shared" si="0"/>
+        <v>0.42666249999999994</v>
+      </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="B38">
         <v>9.11E-2</v>
@@ -8152,42 +11392,46 @@
       </c>
       <c r="I38">
         <v>0.41410000000000002</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="0"/>
+        <v>0.33074999999999993</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B50">
-        <f>AVERAGE(B29:B38)</f>
+        <f t="shared" ref="B50:I50" si="1">AVERAGE(B29:B38)</f>
         <v>0.60258299999999987</v>
       </c>
       <c r="C50">
-        <f>AVERAGE(C29:C38)</f>
+        <f t="shared" si="1"/>
         <v>0.54342749999999995</v>
       </c>
       <c r="D50">
-        <f>AVERAGE(D29:D38)</f>
+        <f t="shared" si="1"/>
         <v>0.69455</v>
       </c>
       <c r="E50">
-        <f>AVERAGE(E29:E38)</f>
+        <f t="shared" si="1"/>
         <v>0.64217999999999997</v>
       </c>
       <c r="F50">
-        <f>AVERAGE(F29:F38)</f>
+        <f t="shared" si="1"/>
         <v>0.57891999999999988</v>
       </c>
       <c r="G50">
-        <f>AVERAGE(G29:G38)</f>
+        <f t="shared" si="1"/>
         <v>0.69531999999999994</v>
       </c>
       <c r="H50">
-        <f>AVERAGE(H29:H38)</f>
+        <f t="shared" si="1"/>
         <v>0.34345999999999999</v>
       </c>
       <c r="I50">
-        <f>AVERAGE(I29:I38)</f>
+        <f t="shared" si="1"/>
         <v>0.70151000000000008</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added New Train Data And New Models
</commit_message>
<xml_diff>
--- a/README_data/Time_Acc_Data.xlsx
+++ b/README_data/Time_Acc_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\SMU\Classes\Spring 2022\CS 3353 (Algorithms)\22s-pa03-girvan-newman-uwunary-tree\README_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E406AA0-9C2A-4F55-AEE2-B7F6F9135948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE90DD96-4AE1-4B6D-85F9-714F2989B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{E3BB0DCF-3EF3-4353-951C-EAD6C2F98100}"/>
   </bookViews>
@@ -5752,7 +5752,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -10438,8 +10437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA28095E-13BC-4864-999E-18B5B8AAC3DA}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated README Images and Data
</commit_message>
<xml_diff>
--- a/README_data/Time_Acc_Data.xlsx
+++ b/README_data/Time_Acc_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\SMU\Classes\Spring 2022\CS 3353 (Algorithms)\22s-pa03-girvan-newman-uwunary-tree\README_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE90DD96-4AE1-4B6D-85F9-714F2989B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056F7A6F-34EA-4A08-B05A-C08F444D4F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{E3BB0DCF-3EF3-4353-951C-EAD6C2F98100}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Dataset</t>
   </si>
@@ -113,6 +113,24 @@
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>128,256,512</t>
+  </si>
+  <si>
+    <t>128,256</t>
+  </si>
+  <si>
+    <t>256,128</t>
+  </si>
+  <si>
+    <t>512,256,128</t>
+  </si>
+  <si>
+    <t>512,1024,512</t>
+  </si>
+  <si>
+    <t>512,256</t>
   </si>
   <si>
     <t>AVG</t>
@@ -460,34 +478,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.96875</c:v>
+                  <c:v>0.89059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.828125</c:v>
+                  <c:v>0.89059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.51559999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39319999999999999</c:v>
+                  <c:v>0.42970000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33300000000000002</c:v>
+                  <c:v>0.3281</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32550000000000001</c:v>
+                  <c:v>0.2969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70299999999999996</c:v>
+                  <c:v>0.77339999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.38279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39839999999999998</c:v>
+                  <c:v>0.4219</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38279999999999997</c:v>
+                  <c:v>0.33589999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,28 +606,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84379999999999999</c:v>
+                  <c:v>0.98440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67190000000000005</c:v>
+                  <c:v>0.90629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46089999999999998</c:v>
+                  <c:v>0.45300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2969</c:v>
+                  <c:v>0.3821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.97660000000000002</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.84379999999999999</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>0.76559999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3594</c:v>
+                  <c:v>0.4375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -704,34 +722,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.99209999999999998</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71879999999999999</c:v>
+                  <c:v>0.88280000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46089999999999998</c:v>
+                  <c:v>0.61699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41410000000000002</c:v>
+                  <c:v>0.42970000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38279999999999997</c:v>
+                  <c:v>0.34379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96089999999999998</c:v>
+                  <c:v>0.98440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.60160000000000002</c:v>
+                  <c:v>0.82809999999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52339999999999998</c:v>
+                  <c:v>0.53910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36720000000000003</c:v>
+                  <c:v>0.3594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,28 +847,28 @@
                   <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3281</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.97660000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.57030000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.46879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3281</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.71089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.33589999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.875</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.57030000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.34379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.34379999999999999</c:v>
@@ -954,28 +972,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89839999999999998</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.74219999999999997</c:v>
+                  <c:v>0.98399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.86719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.42970000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32029999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.97660000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.92190000000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.3281</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.34379999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1074,34 +1092,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.40629999999999999</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3281</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.98440000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.35160000000000002</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.35160000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3281</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.28129999999999999</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.30470000000000003</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.34379999999999999</c:v>
+                  <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39529999999999998</c:v>
+                  <c:v>0.75780000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34379999999999999</c:v>
+                  <c:v>0.36720000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1200,7 +1218,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98399999999999999</c:v>
+                  <c:v>0.98440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -1212,19 +1230,19 @@
                   <c:v>0.63280000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2969</c:v>
+                  <c:v>0.3906</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.375</c:v>
+                  <c:v>0.30470000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80469999999999997</c:v>
+                  <c:v>0.78910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55449999999999999</c:v>
+                  <c:v>0.64059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.41410000000000002</c:v>
@@ -1235,6 +1253,290 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-2FA2-43F4-89BD-72B8E1B0BE4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$29:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98440000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60940000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94530000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67190000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-444B-4534-B105-A6BA16D2081B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$29:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-444B-4534-B105-A6BA16D2081B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,256,128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$29:$L$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30470000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-444B-4534-B105-A6BA16D2081B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,1024,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$29:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92969999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70309999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-444B-4534-B105-A6BA16D2081B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1289,7 +1591,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.49432120184249684"/>
-              <c:y val="0.8399866401575572"/>
+              <c:y val="0.78427188566221007"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1492,22 +1794,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="8"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="9"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="10"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="11"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
         <c:idx val="12"/>
         <c:delete val="1"/>
       </c:legendEntry>
@@ -1521,6 +1807,22 @@
       </c:legendEntry>
       <c:legendEntry>
         <c:idx val="15"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="16"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="17"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="18"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="19"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -1697,21 +1999,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -1864,34 +2151,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.925</c:v>
+                  <c:v>1.964</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.94</c:v>
+                  <c:v>2.089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0497000000000001</c:v>
+                  <c:v>1.92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8979999999999999</c:v>
+                  <c:v>1.9470000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.867</c:v>
+                  <c:v>1.956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.897</c:v>
+                  <c:v>1.9159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.881</c:v>
+                  <c:v>1.9259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8959999999999999</c:v>
+                  <c:v>2.2770000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.028</c:v>
+                  <c:v>2.0990000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8939999999999999</c:v>
+                  <c:v>1.8819999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1971,34 +2258,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.0350000000000001</c:v>
+                  <c:v>1.8819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.028</c:v>
+                  <c:v>1.9359999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9159999999999999</c:v>
+                  <c:v>1.964</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8640000000000001</c:v>
+                  <c:v>1.9330000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9770000000000001</c:v>
+                  <c:v>1.923</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.901</c:v>
+                  <c:v>1.946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.964</c:v>
+                  <c:v>1.889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8560000000000001</c:v>
+                  <c:v>1.871</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.93</c:v>
+                  <c:v>1.9259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.917</c:v>
+                  <c:v>1.9510000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2078,34 +2365,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.998</c:v>
+                  <c:v>1.9139999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9</c:v>
+                  <c:v>2.0339999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.032</c:v>
+                  <c:v>6.6550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.887</c:v>
+                  <c:v>1.946</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.911</c:v>
+                  <c:v>1.9079999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.86</c:v>
+                  <c:v>1.9650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.865</c:v>
+                  <c:v>2.0169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.92</c:v>
+                  <c:v>1.9530000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8440000000000001</c:v>
+                  <c:v>1.8759999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.911</c:v>
+                  <c:v>2.0059999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2185,34 +2472,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.992</c:v>
+                  <c:v>1.905</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9039999999999999</c:v>
+                  <c:v>1.8939999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9259999999999999</c:v>
+                  <c:v>2.012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1389999999999998</c:v>
+                  <c:v>1.9910000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.929</c:v>
+                  <c:v>1.915</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.855</c:v>
+                  <c:v>1.923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.861</c:v>
+                  <c:v>1.9990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8720000000000001</c:v>
+                  <c:v>1.9419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.839</c:v>
+                  <c:v>1.9390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8560000000000001</c:v>
+                  <c:v>2.0329999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2292,34 +2579,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.927</c:v>
+                  <c:v>2.1309999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9770000000000001</c:v>
+                  <c:v>2.0009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9990000000000001</c:v>
+                  <c:v>1.998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.954</c:v>
+                  <c:v>2.0720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.927</c:v>
+                  <c:v>2.0059999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.986</c:v>
+                  <c:v>1.988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9610000000000001</c:v>
+                  <c:v>2.0470000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.903</c:v>
+                  <c:v>2.0030000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9379999999999999</c:v>
+                  <c:v>2.0270000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.978</c:v>
+                  <c:v>2.052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2401,34 +2688,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.954</c:v>
+                  <c:v>2.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9390000000000001</c:v>
+                  <c:v>2.0390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9450000000000001</c:v>
+                  <c:v>2.2250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9750000000000001</c:v>
+                  <c:v>2.0350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8939999999999999</c:v>
+                  <c:v>2.0049999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.958</c:v>
+                  <c:v>2.0249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.913</c:v>
+                  <c:v>2.1269999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1139999999999999</c:v>
+                  <c:v>2.0579999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9350000000000001</c:v>
+                  <c:v>2.0739999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.915</c:v>
+                  <c:v>2.0059999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2510,34 +2797,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.9490000000000001</c:v>
+                  <c:v>2.0720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.077</c:v>
+                  <c:v>2.0209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9259999999999999</c:v>
+                  <c:v>2.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9750000000000001</c:v>
+                  <c:v>2.0830000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9550000000000001</c:v>
+                  <c:v>2.0369999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.946</c:v>
+                  <c:v>2.0910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.946</c:v>
+                  <c:v>2.0659999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9219999999999999</c:v>
+                  <c:v>2.032</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9470000000000001</c:v>
+                  <c:v>2.008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0590000000000002</c:v>
+                  <c:v>2.081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2545,6 +2832,442 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-4CEF-4599-B7C2-8E2567F4EEBE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Dataset 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dataset 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dataset 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dataset 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dataset 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dataset 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dataset 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$16:$J$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0139999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.982</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-504E-4140-80ED-4C7A3B0F19BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Dataset 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dataset 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dataset 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dataset 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dataset 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dataset 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dataset 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$16:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-504E-4140-80ED-4C7A3B0F19BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,256,128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Dataset 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dataset 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dataset 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dataset 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dataset 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dataset 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dataset 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$16:$L$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1960000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0960000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-504E-4140-80ED-4C7A3B0F19BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,1024,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Dataset 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dataset 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Dataset 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Dataset 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Dataset 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Dataset 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Dataset 7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Dataset 8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Dataset 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Dataset 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$16:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.661</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-504E-4140-80ED-4C7A3B0F19BD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2598,8 +3321,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.49216085435518553"/>
-              <c:y val="0.83225987914301391"/>
+              <c:x val="0.48642197343696458"/>
+              <c:y val="0.79505057681743274"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2796,10 +3519,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="8"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2974,21 +3693,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3034,34 +3738,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.925</c:v>
+                  <c:v>1.964</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.94</c:v>
+                  <c:v>2.089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0497000000000001</c:v>
+                  <c:v>1.92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8979999999999999</c:v>
+                  <c:v>1.9470000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.867</c:v>
+                  <c:v>1.956</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.897</c:v>
+                  <c:v>1.9159999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.881</c:v>
+                  <c:v>1.9259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8959999999999999</c:v>
+                  <c:v>2.2770000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.028</c:v>
+                  <c:v>2.0990000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8939999999999999</c:v>
+                  <c:v>1.8819999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3096,21 +3800,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3156,34 +3845,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.0350000000000001</c:v>
+                  <c:v>1.8819999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.028</c:v>
+                  <c:v>1.9359999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9159999999999999</c:v>
+                  <c:v>1.964</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8640000000000001</c:v>
+                  <c:v>1.9330000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9770000000000001</c:v>
+                  <c:v>1.923</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.901</c:v>
+                  <c:v>1.946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.964</c:v>
+                  <c:v>1.889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8560000000000001</c:v>
+                  <c:v>1.871</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.93</c:v>
+                  <c:v>1.9259999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.917</c:v>
+                  <c:v>1.9510000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3218,21 +3907,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3278,34 +3952,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.998</c:v>
+                  <c:v>1.9139999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9</c:v>
+                  <c:v>2.0339999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.032</c:v>
+                  <c:v>6.6550000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.887</c:v>
+                  <c:v>1.946</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.911</c:v>
+                  <c:v>1.9079999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.86</c:v>
+                  <c:v>1.9650000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.865</c:v>
+                  <c:v>2.0169999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.92</c:v>
+                  <c:v>1.9530000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.8440000000000001</c:v>
+                  <c:v>1.8759999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.911</c:v>
+                  <c:v>2.0059999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3340,21 +4014,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent5"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3400,34 +4059,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.992</c:v>
+                  <c:v>1.905</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9039999999999999</c:v>
+                  <c:v>1.8939999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9259999999999999</c:v>
+                  <c:v>2.012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1389999999999998</c:v>
+                  <c:v>1.9910000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.929</c:v>
+                  <c:v>1.915</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.855</c:v>
+                  <c:v>1.923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.861</c:v>
+                  <c:v>1.9990000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.8720000000000001</c:v>
+                  <c:v>1.9419999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.839</c:v>
+                  <c:v>1.9390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8560000000000001</c:v>
+                  <c:v>2.0329999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3462,21 +4121,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent6"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3522,34 +4166,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.927</c:v>
+                  <c:v>2.1309999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9770000000000001</c:v>
+                  <c:v>2.0009999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9990000000000001</c:v>
+                  <c:v>1.998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.954</c:v>
+                  <c:v>2.0720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.927</c:v>
+                  <c:v>2.0059999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.986</c:v>
+                  <c:v>1.988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9610000000000001</c:v>
+                  <c:v>2.0470000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.903</c:v>
+                  <c:v>2.0030000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9379999999999999</c:v>
+                  <c:v>2.0270000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.978</c:v>
+                  <c:v>2.052</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3586,23 +4230,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3648,34 +4275,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.954</c:v>
+                  <c:v>2.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9390000000000001</c:v>
+                  <c:v>2.0390000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9450000000000001</c:v>
+                  <c:v>2.2250000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9750000000000001</c:v>
+                  <c:v>2.0350000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8939999999999999</c:v>
+                  <c:v>2.0049999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.958</c:v>
+                  <c:v>2.0249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.913</c:v>
+                  <c:v>2.1269999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1139999999999999</c:v>
+                  <c:v>2.0579999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9350000000000001</c:v>
+                  <c:v>2.0739999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.915</c:v>
+                  <c:v>2.0059999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3712,23 +4339,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="60000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="movingAvg"/>
-            <c:period val="2"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$16:$A$25</c:f>
@@ -3774,34 +4384,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.9490000000000001</c:v>
+                  <c:v>2.0720000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.077</c:v>
+                  <c:v>2.0209999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.9259999999999999</c:v>
+                  <c:v>2.0609999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9750000000000001</c:v>
+                  <c:v>2.0830000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9550000000000001</c:v>
+                  <c:v>2.0369999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.946</c:v>
+                  <c:v>2.0910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.946</c:v>
+                  <c:v>2.0659999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9219999999999999</c:v>
+                  <c:v>2.032</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9470000000000001</c:v>
+                  <c:v>2.008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0590000000000002</c:v>
+                  <c:v>2.081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3809,6 +4419,288 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-5AB1-4EB6-B3C4-105A101B998B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$16:$J$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.024</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0139999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1219999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.982</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0270000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0099999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-15CF-419B-97E2-C99FEC3471E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$16:$K$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.077</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.0649999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0459999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-15CF-419B-97E2-C99FEC3471E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,256,128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$16:$L$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9970000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0179999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0779999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.056</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.1960000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0960000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-15CF-419B-97E2-C99FEC3471E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,1024,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$16:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.661</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.097</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0369999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.044</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0470000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1339999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.0609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.109</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-15CF-419B-97E2-C99FEC3471E0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3862,8 +4754,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.49216085435518553"/>
-              <c:y val="0.83225987914301391"/>
+              <c:x val="0.49407381466125916"/>
+              <c:y val="0.78760871635231644"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4060,34 +4952,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="7"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="8"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="9"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="10"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="11"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="12"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="13"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4231,9 +5095,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$28:$I$28</c:f>
+              <c:f>Sheet1!$B$28:$M$28</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>GN (80%)</c:v>
                 </c:pt>
@@ -4257,39 +5121,63 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1024,512,256,128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>128,256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128,256,512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>512,256,128</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>512,1024,512</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$50:$I$50</c:f>
+              <c:f>Sheet1!$B$50:$M$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0.60258299999999987</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54342749999999995</c:v>
+                  <c:v>0.52654999999999985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69455</c:v>
+                  <c:v>0.79055000000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64217999999999997</c:v>
+                  <c:v>0.6976500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57891999999999988</c:v>
+                  <c:v>0.65390999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.69531999999999994</c:v>
+                  <c:v>0.84293999999999991</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.34345999999999999</c:v>
+                  <c:v>0.80314000000000019</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70151000000000008</c:v>
+                  <c:v>0.71094000000000013</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.77736000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.73126999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.7968900000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.7336100000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4619,7 +5507,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average Number of Out Edges Vs. Algorithm Accuracy</a:t>
+              <a:t>Average Out</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Degree Count</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Vs. Algorithm Accuracy</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4890,34 +5786,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.96875</c:v>
+                  <c:v>0.89059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.828125</c:v>
+                  <c:v>0.89059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.51559999999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.39319999999999999</c:v>
+                  <c:v>0.42970000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.33300000000000002</c:v>
+                  <c:v>0.3281</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32550000000000001</c:v>
+                  <c:v>0.2969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70299999999999996</c:v>
+                  <c:v>0.77339999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.38279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39839999999999998</c:v>
+                  <c:v>0.4219</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.38279999999999997</c:v>
+                  <c:v>0.33589999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5031,28 +5927,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.84379999999999999</c:v>
+                  <c:v>0.98440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67190000000000005</c:v>
+                  <c:v>0.90629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46089999999999998</c:v>
+                  <c:v>0.45300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.2969</c:v>
+                  <c:v>0.3821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.97660000000000002</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.84379999999999999</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.5</c:v>
+                  <c:v>0.76559999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.3594</c:v>
+                  <c:v>0.4375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5160,34 +6056,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.99209999999999998</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71879999999999999</c:v>
+                  <c:v>0.88280000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46089999999999998</c:v>
+                  <c:v>0.61699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.41410000000000002</c:v>
+                  <c:v>0.42970000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38279999999999997</c:v>
+                  <c:v>0.34379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96089999999999998</c:v>
+                  <c:v>0.98440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.60160000000000002</c:v>
+                  <c:v>0.82809999999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52339999999999998</c:v>
+                  <c:v>0.53910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36720000000000003</c:v>
+                  <c:v>0.3594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5298,28 +6194,28 @@
                   <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.82030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.61719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3281</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.97660000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.57030000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.46879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3281</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>0.71089999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0.33589999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.875</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.57030000000000003</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.34379999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.34379999999999999</c:v>
@@ -5436,28 +6332,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.89839999999999998</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.74219999999999997</c:v>
+                  <c:v>0.98399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.86719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33589999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.42970000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.32029999999999997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.97660000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.92190000000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.3281</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.34379999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5571,34 +6467,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.40629999999999999</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3281</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.98440000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.35160000000000002</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.35160000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.3281</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.28129999999999999</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.30470000000000003</c:v>
+                  <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.34379999999999999</c:v>
+                  <c:v>0.97660000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.39529999999999998</c:v>
+                  <c:v>0.75780000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34379999999999999</c:v>
+                  <c:v>0.36720000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5712,7 +6608,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.98399999999999999</c:v>
+                  <c:v>0.98440000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -5724,19 +6620,19 @@
                   <c:v>0.63280000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2969</c:v>
+                  <c:v>0.3906</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.375</c:v>
+                  <c:v>0.30470000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.99219999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.80469999999999997</c:v>
+                  <c:v>0.78910000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.55449999999999999</c:v>
+                  <c:v>0.64059999999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.41410000000000002</c:v>
@@ -5748,6 +6644,506 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000D-05B5-4D08-B0FD-A390064361C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$29:$J$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98440000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.84379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60940000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.94530000000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67190000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3906</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-49DB-4229-A6B1-402CE4B3ACBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128,256,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$29:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.72660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.97660000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.63280000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34379999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-49DB-4229-A6B1-402CE4B3ACBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,256,128</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$29:$L$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.57030000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.78129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30470000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-49DB-4229-A6B1-402CE4B3ACBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>512,1024,512</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9375</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.859375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.515625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.84375</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$29:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.96879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.35160000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99219999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.92969999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70309999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.42970000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-49DB-4229-A6B1-402CE4B3ACBC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5804,7 +7200,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Average Number Of Out Edges</a:t>
+                  <a:t>Dataset Average Node Out Degree Count</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6008,22 +7404,6 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="8"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="9"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="10"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="11"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:legendEntry>
         <c:idx val="12"/>
         <c:delete val="1"/>
       </c:legendEntry>
@@ -6037,6 +7417,22 @@
       </c:legendEntry>
       <c:legendEntry>
         <c:idx val="15"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="16"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="17"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="18"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="19"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:overlay val="0"/>
@@ -6147,7 +7543,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average Number of Out Edges Vs. Average Accuracy Across</a:t>
+              <a:t>Average Out</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Degree Count</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> Vs. Average Accuracy Across</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -6227,7 +7631,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -6272,39 +7677,39 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$29:$J$38</c:f>
+              <c:f>Sheet1!$N$29:$N$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.91238124999999992</c:v>
+                  <c:v>0.98134166666666678</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88119062500000001</c:v>
+                  <c:v>0.98329166666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71809999999999996</c:v>
+                  <c:v>0.90516666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53873749999999998</c:v>
+                  <c:v>0.73130833333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34338125000000003</c:v>
+                  <c:v>0.48176250000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30533749999999998</c:v>
+                  <c:v>0.32352500000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.84764750000000011</c:v>
+                  <c:v>0.97071500000000011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69825000000000004</c:v>
+                  <c:v>0.86979166666666685</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.42666249999999994</c:v>
+                  <c:v>0.62196666666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.33074999999999993</c:v>
+                  <c:v>0.35395833333333332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6369,7 +7774,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Average Number Of Out Edges</a:t>
+                  <a:t>Dataset Average</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Node Out Degree Count</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9917,16 +11330,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>66674</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>73024</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>44176</xdr:rowOff>
+      <xdr:rowOff>25126</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9953,16 +11366,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>79374</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>155574</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>12699</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:rowOff>69849</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9989,16 +11402,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>492125</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>587375</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>34925</xdr:rowOff>
+      <xdr:rowOff>53975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10027,16 +11440,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>117475</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>174624</xdr:rowOff>
+      <xdr:rowOff>168274</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>112183</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>86783</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:rowOff>126999</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10063,14 +11476,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>53974</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>96307</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>70907</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -10099,14 +11512,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>42333</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>137583</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -10435,10 +11848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA28095E-13BC-4864-999E-18B5B8AAC3DA}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="P13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10451,9 +11864,11 @@
     <col min="6" max="6" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10476,7 +11891,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -10499,7 +11914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -10522,7 +11937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -10545,7 +11960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -10568,7 +11983,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -10591,7 +12006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -10614,7 +12029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -10637,7 +12052,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -10660,7 +12075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -10683,7 +12098,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -10706,41 +12121,54 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="1">
-        <v>256128</v>
-      </c>
-      <c r="H15" s="1">
-        <v>512256</v>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -10748,28 +12176,40 @@
         <v>7.3239999999999998</v>
       </c>
       <c r="C16">
-        <v>1.925</v>
+        <v>1.964</v>
       </c>
       <c r="D16">
-        <v>2.0350000000000001</v>
+        <v>1.8819999999999999</v>
       </c>
       <c r="E16">
-        <v>1.998</v>
+        <v>1.9139999999999999</v>
       </c>
       <c r="F16">
-        <v>1.992</v>
+        <v>1.905</v>
       </c>
       <c r="G16">
-        <v>1.927</v>
+        <v>2.1309999999999998</v>
       </c>
       <c r="H16">
-        <v>1.954</v>
+        <v>2.29</v>
       </c>
       <c r="I16">
-        <v>1.9490000000000001</v>
+        <v>2.0720000000000001</v>
+      </c>
+      <c r="J16">
+        <v>2.008</v>
+      </c>
+      <c r="K16">
+        <v>2.077</v>
+      </c>
+      <c r="L16">
+        <v>2.008</v>
+      </c>
+      <c r="M16">
+        <v>2.661</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -10777,28 +12217,40 @@
         <v>37.32</v>
       </c>
       <c r="C17">
-        <v>1.94</v>
+        <v>2.089</v>
       </c>
       <c r="D17">
-        <v>2.028</v>
+        <v>1.9359999999999999</v>
       </c>
       <c r="E17">
-        <v>1.9</v>
+        <v>2.0339999999999998</v>
       </c>
       <c r="F17">
-        <v>1.9039999999999999</v>
+        <v>1.8939999999999999</v>
       </c>
       <c r="G17">
-        <v>1.9770000000000001</v>
+        <v>2.0009999999999999</v>
       </c>
       <c r="H17">
-        <v>1.9390000000000001</v>
+        <v>2.0390000000000001</v>
       </c>
       <c r="I17">
-        <v>2.077</v>
+        <v>2.0209999999999999</v>
+      </c>
+      <c r="J17">
+        <v>2.024</v>
+      </c>
+      <c r="K17">
+        <v>2.056</v>
+      </c>
+      <c r="L17">
+        <v>1.9970000000000001</v>
+      </c>
+      <c r="M17">
+        <v>2.097</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -10806,28 +12258,40 @@
         <v>38.468699999999998</v>
       </c>
       <c r="C18">
-        <v>2.0497000000000001</v>
+        <v>1.92</v>
       </c>
       <c r="D18">
-        <v>1.9159999999999999</v>
+        <v>1.964</v>
       </c>
       <c r="E18">
-        <v>2.032</v>
+        <v>6.6550000000000002</v>
       </c>
       <c r="F18">
-        <v>1.9259999999999999</v>
+        <v>2.012</v>
       </c>
       <c r="G18">
-        <v>1.9990000000000001</v>
+        <v>1.998</v>
       </c>
       <c r="H18">
-        <v>1.9450000000000001</v>
+        <v>2.2250000000000001</v>
       </c>
       <c r="I18">
-        <v>1.9259999999999999</v>
+        <v>2.0609999999999999</v>
+      </c>
+      <c r="J18">
+        <v>2.056</v>
+      </c>
+      <c r="K18">
+        <v>2.0459999999999998</v>
+      </c>
+      <c r="L18">
+        <v>1.994</v>
+      </c>
+      <c r="M18">
+        <v>2.0369999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -10835,28 +12299,40 @@
         <v>43.039000000000001</v>
       </c>
       <c r="C19">
-        <v>1.8979999999999999</v>
+        <v>1.9470000000000001</v>
       </c>
       <c r="D19">
-        <v>1.8640000000000001</v>
+        <v>1.9330000000000001</v>
       </c>
       <c r="E19">
-        <v>1.887</v>
+        <v>1.946</v>
       </c>
       <c r="F19">
-        <v>2.1389999999999998</v>
+        <v>1.9910000000000001</v>
       </c>
       <c r="G19">
-        <v>1.954</v>
+        <v>2.0720000000000001</v>
       </c>
       <c r="H19">
-        <v>1.9750000000000001</v>
+        <v>2.0350000000000001</v>
       </c>
       <c r="I19">
-        <v>1.9750000000000001</v>
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="J19">
+        <v>2.0139999999999998</v>
+      </c>
+      <c r="K19">
+        <v>2.0459999999999998</v>
+      </c>
+      <c r="L19">
+        <v>2.0529999999999999</v>
+      </c>
+      <c r="M19">
+        <v>2.0369999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -10864,28 +12340,40 @@
         <v>33.281999999999996</v>
       </c>
       <c r="C20">
-        <v>1.867</v>
+        <v>1.956</v>
       </c>
       <c r="D20">
-        <v>1.9770000000000001</v>
+        <v>1.923</v>
       </c>
       <c r="E20">
-        <v>1.911</v>
+        <v>1.9079999999999999</v>
       </c>
       <c r="F20">
-        <v>1.929</v>
+        <v>1.915</v>
       </c>
       <c r="G20">
-        <v>1.927</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="H20">
-        <v>1.8939999999999999</v>
+        <v>2.0049999999999999</v>
       </c>
       <c r="I20">
-        <v>1.9550000000000001</v>
+        <v>2.0369999999999999</v>
+      </c>
+      <c r="J20">
+        <v>2.004</v>
+      </c>
+      <c r="K20">
+        <v>2.25</v>
+      </c>
+      <c r="L20">
+        <v>2.0179999999999998</v>
+      </c>
+      <c r="M20">
+        <v>2.129</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -10893,28 +12381,40 @@
         <v>34.5</v>
       </c>
       <c r="C21">
-        <v>1.897</v>
+        <v>1.9159999999999999</v>
       </c>
       <c r="D21">
-        <v>1.901</v>
+        <v>1.946</v>
       </c>
       <c r="E21">
-        <v>1.86</v>
+        <v>1.9650000000000001</v>
       </c>
       <c r="F21">
-        <v>1.855</v>
+        <v>1.923</v>
       </c>
       <c r="G21">
-        <v>1.986</v>
+        <v>1.988</v>
       </c>
       <c r="H21">
-        <v>1.958</v>
+        <v>2.0249999999999999</v>
       </c>
       <c r="I21">
-        <v>1.946</v>
+        <v>2.0910000000000002</v>
+      </c>
+      <c r="J21">
+        <v>2.1219999999999999</v>
+      </c>
+      <c r="K21">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="L21">
+        <v>2.0750000000000002</v>
+      </c>
+      <c r="M21">
+        <v>2.044</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -10922,28 +12422,40 @@
         <v>36.298699999999997</v>
       </c>
       <c r="C22">
-        <v>1.881</v>
+        <v>1.9259999999999999</v>
       </c>
       <c r="D22">
-        <v>1.964</v>
+        <v>1.889</v>
       </c>
       <c r="E22">
-        <v>1.865</v>
+        <v>2.0169999999999999</v>
       </c>
       <c r="F22">
-        <v>1.861</v>
+        <v>1.9990000000000001</v>
       </c>
       <c r="G22">
-        <v>1.9610000000000001</v>
+        <v>2.0470000000000002</v>
       </c>
       <c r="H22">
-        <v>1.913</v>
+        <v>2.1269999999999998</v>
       </c>
       <c r="I22">
-        <v>1.946</v>
+        <v>2.0659999999999998</v>
+      </c>
+      <c r="J22">
+        <v>1.9850000000000001</v>
+      </c>
+      <c r="K22">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="L22">
+        <v>2.0779999999999998</v>
+      </c>
+      <c r="M22">
+        <v>2.0470000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -10951,28 +12463,40 @@
         <v>44.28</v>
       </c>
       <c r="C23">
-        <v>1.8959999999999999</v>
+        <v>2.2770000000000001</v>
       </c>
       <c r="D23">
-        <v>1.8560000000000001</v>
+        <v>1.871</v>
       </c>
       <c r="E23">
-        <v>1.92</v>
+        <v>1.9530000000000001</v>
       </c>
       <c r="F23">
-        <v>1.8720000000000001</v>
+        <v>1.9419999999999999</v>
       </c>
       <c r="G23">
-        <v>1.903</v>
+        <v>2.0030000000000001</v>
       </c>
       <c r="H23">
-        <v>2.1139999999999999</v>
+        <v>2.0579999999999998</v>
       </c>
       <c r="I23">
-        <v>1.9219999999999999</v>
+        <v>2.032</v>
+      </c>
+      <c r="J23">
+        <v>1.982</v>
+      </c>
+      <c r="K23">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="L23">
+        <v>2.056</v>
+      </c>
+      <c r="M23">
+        <v>2.1339999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -10980,28 +12504,40 @@
         <v>33.74</v>
       </c>
       <c r="C24">
-        <v>2.028</v>
+        <v>2.0990000000000002</v>
       </c>
       <c r="D24">
-        <v>1.93</v>
+        <v>1.9259999999999999</v>
       </c>
       <c r="E24">
-        <v>1.8440000000000001</v>
+        <v>1.8759999999999999</v>
       </c>
       <c r="F24">
-        <v>1.839</v>
+        <v>1.9390000000000001</v>
       </c>
       <c r="G24">
-        <v>1.9379999999999999</v>
+        <v>2.0270000000000001</v>
       </c>
       <c r="H24">
-        <v>1.9350000000000001</v>
+        <v>2.0739999999999998</v>
       </c>
       <c r="I24">
-        <v>1.9470000000000001</v>
+        <v>2.008</v>
+      </c>
+      <c r="J24">
+        <v>2.0270000000000001</v>
+      </c>
+      <c r="K24">
+        <v>2.0459999999999998</v>
+      </c>
+      <c r="L24">
+        <v>2.1960000000000002</v>
+      </c>
+      <c r="M24">
+        <v>2.0609999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -11009,33 +12545,45 @@
         <v>37.659999999999997</v>
       </c>
       <c r="C25">
-        <v>1.8939999999999999</v>
+        <v>1.8819999999999999</v>
       </c>
       <c r="D25">
-        <v>1.917</v>
+        <v>1.9510000000000001</v>
       </c>
       <c r="E25">
-        <v>1.911</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="F25">
-        <v>1.8560000000000001</v>
+        <v>2.0329999999999999</v>
       </c>
       <c r="G25">
-        <v>1.978</v>
+        <v>2.052</v>
       </c>
       <c r="H25">
-        <v>1.915</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="I25">
-        <v>2.0590000000000002</v>
+        <v>2.081</v>
+      </c>
+      <c r="J25">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="K25">
+        <v>2.0459999999999998</v>
+      </c>
+      <c r="L25">
+        <v>2.0960000000000001</v>
+      </c>
+      <c r="M25">
+        <v>2.109</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -11057,17 +12605,29 @@
       <c r="G28" s="1">
         <v>256128</v>
       </c>
-      <c r="H28" s="1">
-        <v>512256</v>
+      <c r="H28" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="L28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>14</v>
       </c>
@@ -11075,13 +12635,13 @@
         <v>0.9869</v>
       </c>
       <c r="C29">
-        <v>0.96875</v>
+        <v>0.89059999999999995</v>
       </c>
       <c r="D29">
         <v>0.99219999999999997</v>
       </c>
       <c r="E29">
-        <v>0.99209999999999998</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="F29">
         <v>0.97660000000000002</v>
@@ -11090,17 +12650,29 @@
         <v>0.99219999999999997</v>
       </c>
       <c r="H29">
-        <v>0.40629999999999999</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="I29">
-        <v>0.98399999999999999</v>
+        <v>0.98440000000000005</v>
       </c>
       <c r="J29">
-        <f>AVERAGE(B29:I29)</f>
-        <v>0.91238124999999992</v>
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="K29">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="L29">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="M29">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ref="N17:N38" si="0">AVERAGE(B29:M29)</f>
+        <v>0.98134166666666678</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -11108,7 +12680,7 @@
         <v>0.91669999999999996</v>
       </c>
       <c r="C30">
-        <v>0.828125</v>
+        <v>0.89059999999999995</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -11117,23 +12689,35 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>0.97660000000000002</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
       <c r="H30">
-        <v>0.3281</v>
+        <v>1</v>
       </c>
       <c r="I30">
         <v>1</v>
       </c>
       <c r="J30">
-        <f t="shared" ref="J30:J38" si="0">AVERAGE(B30:I30)</f>
-        <v>0.88119062500000001</v>
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="0"/>
+        <v>0.98329166666666667</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -11141,32 +12725,44 @@
         <v>0.83850000000000002</v>
       </c>
       <c r="C31">
-        <v>0.5625</v>
+        <v>0.51559999999999995</v>
       </c>
       <c r="D31">
-        <v>0.84379999999999999</v>
+        <v>0.98440000000000005</v>
       </c>
       <c r="E31">
-        <v>0.71879999999999999</v>
+        <v>0.88280000000000003</v>
       </c>
       <c r="F31">
-        <v>0.57030000000000003</v>
+        <v>0.82030000000000003</v>
       </c>
       <c r="G31">
-        <v>0.89839999999999998</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="H31">
-        <v>0.35160000000000002</v>
+        <v>0.98440000000000005</v>
       </c>
       <c r="I31">
         <v>0.96089999999999998</v>
       </c>
       <c r="J31">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="K31">
+        <v>0.9375</v>
+      </c>
+      <c r="L31">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="M31">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="N31">
         <f t="shared" si="0"/>
-        <v>0.71809999999999996</v>
+        <v>0.90516666666666667</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -11174,32 +12770,44 @@
         <v>0.58850000000000002</v>
       </c>
       <c r="C32">
-        <v>0.39319999999999999</v>
+        <v>0.42970000000000003</v>
       </c>
       <c r="D32">
-        <v>0.67190000000000005</v>
+        <v>0.90629999999999999</v>
       </c>
       <c r="E32">
-        <v>0.46089999999999998</v>
+        <v>0.61699999999999999</v>
       </c>
       <c r="F32">
-        <v>0.46879999999999999</v>
+        <v>0.61719999999999997</v>
       </c>
       <c r="G32">
-        <v>0.74219999999999997</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="H32">
-        <v>0.35160000000000002</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="I32">
         <v>0.63280000000000003</v>
       </c>
       <c r="J32">
+        <v>0.84379999999999999</v>
+      </c>
+      <c r="K32">
+        <v>0.72660000000000002</v>
+      </c>
+      <c r="L32">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="M32">
+        <v>0.46879999999999999</v>
+      </c>
+      <c r="N32">
         <f t="shared" si="0"/>
-        <v>0.53873749999999998</v>
+        <v>0.73130833333333334</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -11207,32 +12815,44 @@
         <v>0.15625</v>
       </c>
       <c r="C33">
-        <v>0.33300000000000002</v>
+        <v>0.3281</v>
       </c>
       <c r="D33">
-        <v>0.46089999999999998</v>
+        <v>0.45300000000000001</v>
       </c>
       <c r="E33">
-        <v>0.41410000000000002</v>
+        <v>0.42970000000000003</v>
       </c>
       <c r="F33">
-        <v>0.3281</v>
+        <v>0.42970000000000003</v>
       </c>
       <c r="G33">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="H33">
+        <v>0.61719999999999997</v>
+      </c>
+      <c r="I33">
+        <v>0.3906</v>
+      </c>
+      <c r="J33">
+        <v>0.60940000000000005</v>
+      </c>
+      <c r="K33">
         <v>0.42970000000000003</v>
       </c>
-      <c r="H33">
-        <v>0.3281</v>
-      </c>
-      <c r="I33">
-        <v>0.2969</v>
-      </c>
-      <c r="J33">
+      <c r="L33">
+        <v>0.57030000000000003</v>
+      </c>
+      <c r="M33">
+        <v>0.5</v>
+      </c>
+      <c r="N33">
         <f t="shared" si="0"/>
-        <v>0.34338125000000003</v>
+        <v>0.48176250000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -11240,32 +12860,44 @@
         <v>0.125</v>
       </c>
       <c r="C34">
-        <v>0.32550000000000001</v>
+        <v>0.2969</v>
       </c>
       <c r="D34">
-        <v>0.2969</v>
+        <v>0.3821</v>
       </c>
       <c r="E34">
-        <v>0.38279999999999997</v>
+        <v>0.34379999999999999</v>
       </c>
       <c r="F34">
+        <v>0.3281</v>
+      </c>
+      <c r="G34">
         <v>0.33589999999999998</v>
       </c>
-      <c r="G34">
-        <v>0.32029999999999997</v>
-      </c>
       <c r="H34">
-        <v>0.28129999999999999</v>
+        <v>0.35160000000000002</v>
       </c>
       <c r="I34">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="J34">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="K34">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="L34">
         <v>0.375</v>
       </c>
-      <c r="J34">
+      <c r="M34">
+        <v>0.35160000000000002</v>
+      </c>
+      <c r="N34">
         <f t="shared" si="0"/>
-        <v>0.30533749999999998</v>
+        <v>0.32352500000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -11273,32 +12905,44 @@
         <v>0.99217999999999995</v>
       </c>
       <c r="C35">
-        <v>0.70299999999999996</v>
+        <v>0.77339999999999998</v>
       </c>
       <c r="D35">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="E35">
+        <v>0.98440000000000005</v>
+      </c>
+      <c r="F35">
         <v>0.97660000000000002</v>
       </c>
-      <c r="E35">
-        <v>0.96089999999999998</v>
-      </c>
-      <c r="F35">
-        <v>0.875</v>
-      </c>
       <c r="G35">
-        <v>0.97660000000000002</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="H35">
-        <v>0.30470000000000003</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="I35">
         <v>0.99219999999999997</v>
       </c>
       <c r="J35">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="K35">
+        <v>0.97660000000000002</v>
+      </c>
+      <c r="L35">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="M35">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="N35">
         <f t="shared" si="0"/>
-        <v>0.84764750000000011</v>
+        <v>0.97071500000000011</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -11306,32 +12950,44 @@
         <v>0.96089999999999998</v>
       </c>
       <c r="C36">
-        <v>0.53900000000000003</v>
+        <v>0.38279999999999997</v>
       </c>
       <c r="D36">
-        <v>0.84379999999999999</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="E36">
-        <v>0.60160000000000002</v>
+        <v>0.82809999999999995</v>
       </c>
       <c r="F36">
-        <v>0.57030000000000003</v>
+        <v>0.71089999999999998</v>
       </c>
       <c r="G36">
-        <v>0.92190000000000005</v>
+        <v>0.99219999999999997</v>
       </c>
       <c r="H36">
-        <v>0.34379999999999999</v>
+        <v>0.97660000000000002</v>
       </c>
       <c r="I36">
-        <v>0.80469999999999997</v>
+        <v>0.78910000000000002</v>
       </c>
       <c r="J36">
+        <v>0.94530000000000003</v>
+      </c>
+      <c r="K36">
+        <v>0.9375</v>
+      </c>
+      <c r="L36">
+        <v>0.99219999999999997</v>
+      </c>
+      <c r="M36">
+        <v>0.92969999999999997</v>
+      </c>
+      <c r="N36">
         <f t="shared" si="0"/>
-        <v>0.69825000000000004</v>
+        <v>0.86979166666666685</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -11339,32 +12995,44 @@
         <v>0.36980000000000002</v>
       </c>
       <c r="C37">
-        <v>0.39839999999999998</v>
+        <v>0.4219</v>
       </c>
       <c r="D37">
-        <v>0.5</v>
+        <v>0.76559999999999995</v>
       </c>
       <c r="E37">
-        <v>0.52339999999999998</v>
+        <v>0.53910000000000002</v>
       </c>
       <c r="F37">
-        <v>0.34379999999999999</v>
+        <v>0.33589999999999998</v>
       </c>
       <c r="G37">
-        <v>0.3281</v>
+        <v>0.84379999999999999</v>
       </c>
       <c r="H37">
-        <v>0.39529999999999998</v>
+        <v>0.75780000000000003</v>
       </c>
       <c r="I37">
-        <v>0.55449999999999999</v>
+        <v>0.64059999999999995</v>
       </c>
       <c r="J37">
+        <v>0.67190000000000005</v>
+      </c>
+      <c r="K37">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="L37">
+        <v>0.78129999999999999</v>
+      </c>
+      <c r="M37">
+        <v>0.70309999999999995</v>
+      </c>
+      <c r="N37">
         <f t="shared" si="0"/>
-        <v>0.42666249999999994</v>
+        <v>0.62196666666666667</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>23</v>
       </c>
@@ -11372,66 +13040,94 @@
         <v>9.11E-2</v>
       </c>
       <c r="C38">
-        <v>0.38279999999999997</v>
+        <v>0.33589999999999998</v>
       </c>
       <c r="D38">
+        <v>0.4375</v>
+      </c>
+      <c r="E38">
         <v>0.3594</v>
-      </c>
-      <c r="E38">
-        <v>0.36720000000000003</v>
       </c>
       <c r="F38">
         <v>0.34379999999999999</v>
       </c>
       <c r="G38">
-        <v>0.34379999999999999</v>
+        <v>0.42970000000000003</v>
       </c>
       <c r="H38">
-        <v>0.34379999999999999</v>
+        <v>0.36720000000000003</v>
       </c>
       <c r="I38">
         <v>0.41410000000000002</v>
       </c>
       <c r="J38">
+        <v>0.3906</v>
+      </c>
+      <c r="K38">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="L38">
+        <v>0.30470000000000003</v>
+      </c>
+      <c r="M38">
+        <v>0.42970000000000003</v>
+      </c>
+      <c r="N38">
         <f t="shared" si="0"/>
-        <v>0.33074999999999993</v>
+        <v>0.35395833333333332</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>24</v>
       </c>
       <c r="B50">
-        <f t="shared" ref="B50:I50" si="1">AVERAGE(B29:B38)</f>
+        <f t="shared" ref="B50:M50" si="1">AVERAGE(B29:B38)</f>
         <v>0.60258299999999987</v>
       </c>
       <c r="C50">
-        <f t="shared" si="1"/>
-        <v>0.54342749999999995</v>
+        <f>AVERAGE(C29:C38)</f>
+        <v>0.52654999999999985</v>
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
-        <v>0.69455</v>
+        <v>0.79055000000000009</v>
       </c>
       <c r="E50">
         <f t="shared" si="1"/>
-        <v>0.64217999999999997</v>
+        <v>0.6976500000000001</v>
       </c>
       <c r="F50">
         <f t="shared" si="1"/>
-        <v>0.57891999999999988</v>
+        <v>0.65390999999999999</v>
       </c>
       <c r="G50">
+        <f>AVERAGE(G29:G38)</f>
+        <v>0.84293999999999991</v>
+      </c>
+      <c r="H50">
+        <f>AVERAGE(H29:H38)</f>
+        <v>0.80314000000000019</v>
+      </c>
+      <c r="I50">
+        <f>AVERAGE(I29:I38)</f>
+        <v>0.71094000000000013</v>
+      </c>
+      <c r="J50">
         <f t="shared" si="1"/>
-        <v>0.69531999999999994</v>
-      </c>
-      <c r="H50">
+        <v>0.77736000000000005</v>
+      </c>
+      <c r="K50">
         <f t="shared" si="1"/>
-        <v>0.34345999999999999</v>
-      </c>
-      <c r="I50">
+        <v>0.73126999999999998</v>
+      </c>
+      <c r="L50">
         <f t="shared" si="1"/>
-        <v>0.70151000000000008</v>
+        <v>0.7968900000000001</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="1"/>
+        <v>0.7336100000000001</v>
       </c>
     </row>
     <row r="70" spans="7:9" x14ac:dyDescent="0.35">

</xml_diff>